<commit_message>
Practice-06 Image-05 Defining Service Lifecycles
</commit_message>
<xml_diff>
--- a/Excell/A1.xlsx
+++ b/Excell/A1.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="139">
   <si>
     <t>Number</t>
   </si>
@@ -415,6 +415,59 @@
   </si>
   <si>
     <t>bathtub (n.) AM</t>
+  </si>
+  <si>
+    <t>bathroom (n.)</t>
+  </si>
+  <si>
+    <t>حمام</t>
+  </si>
+  <si>
+    <t>be (v. aux v.)</t>
+  </si>
+  <si>
+    <t>present tense:
+I am
+you are
+he/she/it is
+we are
+you are
+they are
+--------
+past tense:
+I was
+you were
+he/she/it was
+we were
+you were
+they were
+---------
+present participle:
+being
+---------
+past participle:
+been</t>
+  </si>
+  <si>
+    <t>بودن</t>
+  </si>
+  <si>
+    <t>beach (n.)</t>
+  </si>
+  <si>
+    <t>ساحل</t>
+  </si>
+  <si>
+    <t>beautiful (adj.)</t>
+  </si>
+  <si>
+    <t>زیبا</t>
+  </si>
+  <si>
+    <t>because (conj.)</t>
+  </si>
+  <si>
+    <t>زیرا</t>
   </si>
 </sst>
 </file>
@@ -2779,7 +2832,7 @@
     </row>
     <row r="59">
       <c r="A59" s="1"/>
-      <c r="B59" s="7" t="s">
+      <c r="B59" s="13" t="s">
         <v>127</v>
       </c>
       <c r="C59" s="19"/>
@@ -2811,9 +2864,13 @@
     </row>
     <row r="60">
       <c r="A60" s="1"/>
-      <c r="B60" s="20"/>
+      <c r="B60" s="7" t="s">
+        <v>128</v>
+      </c>
       <c r="C60" s="19"/>
-      <c r="D60" s="12"/>
+      <c r="D60" s="9" t="s">
+        <v>129</v>
+      </c>
       <c r="E60" s="12"/>
       <c r="F60" s="6"/>
       <c r="G60" s="6"/>
@@ -2839,9 +2896,15 @@
     </row>
     <row r="61">
       <c r="A61" s="1"/>
-      <c r="B61" s="20"/>
-      <c r="C61" s="19"/>
-      <c r="D61" s="12"/>
+      <c r="B61" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="C61" s="8" t="s">
+        <v>131</v>
+      </c>
+      <c r="D61" s="9" t="s">
+        <v>132</v>
+      </c>
       <c r="E61" s="12"/>
       <c r="F61" s="6"/>
       <c r="G61" s="6"/>
@@ -2867,9 +2930,13 @@
     </row>
     <row r="62">
       <c r="A62" s="1"/>
-      <c r="B62" s="20"/>
+      <c r="B62" s="7" t="s">
+        <v>133</v>
+      </c>
       <c r="C62" s="19"/>
-      <c r="D62" s="12"/>
+      <c r="D62" s="9" t="s">
+        <v>134</v>
+      </c>
       <c r="E62" s="12"/>
       <c r="F62" s="6"/>
       <c r="G62" s="6"/>
@@ -2895,9 +2962,13 @@
     </row>
     <row r="63">
       <c r="A63" s="1"/>
-      <c r="B63" s="20"/>
+      <c r="B63" s="7" t="s">
+        <v>135</v>
+      </c>
       <c r="C63" s="19"/>
-      <c r="D63" s="12"/>
+      <c r="D63" s="9" t="s">
+        <v>136</v>
+      </c>
       <c r="E63" s="12"/>
       <c r="F63" s="6"/>
       <c r="G63" s="6"/>
@@ -2923,9 +2994,13 @@
     </row>
     <row r="64">
       <c r="A64" s="1"/>
-      <c r="B64" s="20"/>
+      <c r="B64" s="7" t="s">
+        <v>137</v>
+      </c>
       <c r="C64" s="19"/>
-      <c r="D64" s="12"/>
+      <c r="D64" s="9" t="s">
+        <v>138</v>
+      </c>
       <c r="E64" s="12"/>
       <c r="F64" s="6"/>
       <c r="G64" s="6"/>

</xml_diff>